<commit_message>
Latest Code for Bulk upload
</commit_message>
<xml_diff>
--- a/src/Data/AutomationInputSheet_Phase 2ARegressionJetUI.XLSX
+++ b/src/Data/AutomationInputSheet_Phase 2ARegressionJetUI.XLSX
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StandardandProductized" sheetId="1" r:id="rId1"/>
     <sheet name="ContainerNewandModify" sheetId="2" r:id="rId2"/>
+    <sheet name="Bulk" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">StandardandProductized!$F$1:$F$82</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="210">
   <si>
     <t>Product</t>
   </si>
@@ -618,9 +619,6 @@
     <t>Promotions</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Execution Required (Yes/No)</t>
   </si>
   <si>
@@ -664,6 +662,12 @@
   </si>
   <si>
     <t>QTO CPQ and non CPQ supported  products- Container Modify</t>
+  </si>
+  <si>
+    <t>Line Level &gt; Percentage Off</t>
+  </si>
+  <si>
+    <t>Bulk Upload</t>
   </si>
 </sst>
 </file>
@@ -801,7 +805,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -908,22 +912,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -936,21 +925,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -960,6 +949,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1270,10 +1277,10 @@
   <dimension ref="A1:XEJ85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,40 +1317,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
     </row>
     <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -1447,19 +1454,19 @@
       </c>
     </row>
     <row r="3" spans="1:33" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -1506,7 +1513,7 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="15"/>
-      <c r="AB3" s="42" t="s">
+      <c r="AB3" s="47" t="s">
         <v>179</v>
       </c>
       <c r="AC3" s="22" t="s">
@@ -1523,13 +1530,13 @@
       </c>
     </row>
     <row r="4" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="15" t="s">
         <v>31</v>
       </c>
@@ -1576,7 +1583,7 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
-      <c r="AB4" s="42"/>
+      <c r="AB4" s="47"/>
       <c r="AC4" s="22" t="s">
         <v>39</v>
       </c>
@@ -1591,13 +1598,13 @@
       </c>
     </row>
     <row r="5" spans="1:33" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1640,7 +1647,7 @@
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
       <c r="AA5" s="15"/>
-      <c r="AB5" s="42"/>
+      <c r="AB5" s="47"/>
       <c r="AC5" s="22" t="s">
         <v>39</v>
       </c>
@@ -1655,13 +1662,13 @@
       </c>
     </row>
     <row r="6" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="15" t="s">
         <v>118</v>
       </c>
@@ -1710,7 +1717,7 @@
       <c r="Y6" s="15"/>
       <c r="Z6" s="15"/>
       <c r="AA6" s="15"/>
-      <c r="AB6" s="42"/>
+      <c r="AB6" s="47"/>
       <c r="AC6" s="22" t="s">
         <v>39</v>
       </c>
@@ -1725,19 +1732,19 @@
       </c>
     </row>
     <row r="7" spans="1:33" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="15" t="s">
@@ -1784,7 +1791,7 @@
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
       <c r="AA7" s="15"/>
-      <c r="AB7" s="42" t="s">
+      <c r="AB7" s="47" t="s">
         <v>179</v>
       </c>
       <c r="AC7" s="22" t="s">
@@ -1801,13 +1808,13 @@
       </c>
     </row>
     <row r="8" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
@@ -1852,7 +1859,7 @@
       <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
       <c r="AA8" s="15"/>
-      <c r="AB8" s="42"/>
+      <c r="AB8" s="47"/>
       <c r="AC8" s="22" t="s">
         <v>39</v>
       </c>
@@ -1867,13 +1874,13 @@
       </c>
     </row>
     <row r="9" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1918,7 +1925,7 @@
       <c r="Y9" s="15"/>
       <c r="Z9" s="15"/>
       <c r="AA9" s="15"/>
-      <c r="AB9" s="42"/>
+      <c r="AB9" s="47"/>
       <c r="AC9" s="22" t="s">
         <v>39</v>
       </c>
@@ -1933,13 +1940,13 @@
       </c>
     </row>
     <row r="10" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="15" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +1991,7 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
       <c r="AA10" s="15"/>
-      <c r="AB10" s="42"/>
+      <c r="AB10" s="47"/>
       <c r="AC10" s="22" t="s">
         <v>39</v>
       </c>
@@ -1999,19 +2006,19 @@
       </c>
     </row>
     <row r="11" spans="1:33" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="15" t="s">
@@ -2060,7 +2067,7 @@
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
       <c r="AA11" s="15"/>
-      <c r="AB11" s="42" t="s">
+      <c r="AB11" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="22" t="s">
@@ -2077,13 +2084,13 @@
       </c>
     </row>
     <row r="12" spans="1:33" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="15" t="s">
         <v>31</v>
       </c>
@@ -2130,7 +2137,7 @@
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="42"/>
+      <c r="AB12" s="47"/>
       <c r="AC12" s="22" t="s">
         <v>39</v>
       </c>
@@ -2145,13 +2152,13 @@
       </c>
     </row>
     <row r="13" spans="1:33" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="15" t="s">
         <v>31</v>
       </c>
@@ -2198,7 +2205,7 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="15"/>
-      <c r="AB13" s="42"/>
+      <c r="AB13" s="47"/>
       <c r="AC13" s="22" t="s">
         <v>39</v>
       </c>
@@ -2213,13 +2220,13 @@
       </c>
     </row>
     <row r="14" spans="1:33" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="15" t="s">
         <v>31</v>
       </c>
@@ -2266,7 +2273,7 @@
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
       <c r="AA14" s="15"/>
-      <c r="AB14" s="42"/>
+      <c r="AB14" s="47"/>
       <c r="AC14" s="22" t="s">
         <v>39</v>
       </c>
@@ -2281,19 +2288,19 @@
       </c>
     </row>
     <row r="15" spans="1:33" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -2338,7 +2345,7 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
       <c r="AA15" s="15"/>
-      <c r="AB15" s="42" t="s">
+      <c r="AB15" s="47" t="s">
         <v>179</v>
       </c>
       <c r="AC15" s="22" t="s">
@@ -2355,13 +2362,13 @@
       </c>
     </row>
     <row r="16" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="15" t="s">
         <v>27</v>
       </c>
@@ -2404,7 +2411,7 @@
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
       <c r="AA16" s="15"/>
-      <c r="AB16" s="42"/>
+      <c r="AB16" s="47"/>
       <c r="AC16" s="22" t="s">
         <v>39</v>
       </c>
@@ -2419,19 +2426,19 @@
       </c>
     </row>
     <row r="17" spans="1:32" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F17" s="15" t="s">
@@ -2482,7 +2489,7 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
       <c r="AA17" s="15"/>
-      <c r="AB17" s="42" t="s">
+      <c r="AB17" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC17" s="22" t="s">
@@ -2499,13 +2506,13 @@
       </c>
     </row>
     <row r="18" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="15" t="s">
         <v>118</v>
       </c>
@@ -2554,7 +2561,7 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
       <c r="AA18" s="15"/>
-      <c r="AB18" s="42"/>
+      <c r="AB18" s="47"/>
       <c r="AC18" s="22" t="s">
         <v>39</v>
       </c>
@@ -2569,13 +2576,13 @@
       </c>
     </row>
     <row r="19" spans="1:32" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="15" t="s">
         <v>118</v>
       </c>
@@ -2624,7 +2631,7 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
       <c r="AA19" s="15"/>
-      <c r="AB19" s="42"/>
+      <c r="AB19" s="47"/>
       <c r="AC19" s="22" t="s">
         <v>39</v>
       </c>
@@ -2639,13 +2646,13 @@
       </c>
     </row>
     <row r="20" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="15" t="s">
         <v>118</v>
       </c>
@@ -2694,7 +2701,7 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
       <c r="AA20" s="15"/>
-      <c r="AB20" s="42"/>
+      <c r="AB20" s="47"/>
       <c r="AC20" s="22" t="s">
         <v>39</v>
       </c>
@@ -2709,19 +2716,19 @@
       </c>
     </row>
     <row r="21" spans="1:32" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="15" t="s">
@@ -2764,7 +2771,7 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
       <c r="AA21" s="15"/>
-      <c r="AB21" s="42" t="s">
+      <c r="AB21" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC21" s="22" t="s">
@@ -2781,13 +2788,13 @@
       </c>
     </row>
     <row r="22" spans="1:32" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="42"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="15" t="s">
         <v>118</v>
       </c>
@@ -2836,7 +2843,7 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
       <c r="AA22" s="15"/>
-      <c r="AB22" s="42"/>
+      <c r="AB22" s="47"/>
       <c r="AC22" s="22" t="s">
         <v>39</v>
       </c>
@@ -2851,13 +2858,13 @@
       </c>
     </row>
     <row r="23" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="15" t="s">
         <v>118</v>
       </c>
@@ -2906,7 +2913,7 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
       <c r="AA23" s="15"/>
-      <c r="AB23" s="42"/>
+      <c r="AB23" s="47"/>
       <c r="AC23" s="22" t="s">
         <v>39</v>
       </c>
@@ -2921,13 +2928,13 @@
       </c>
     </row>
     <row r="24" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="15" t="s">
         <v>118</v>
       </c>
@@ -2976,7 +2983,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
       <c r="AA24" s="15"/>
-      <c r="AB24" s="42"/>
+      <c r="AB24" s="47"/>
       <c r="AC24" s="22" t="s">
         <v>39</v>
       </c>
@@ -2991,13 +2998,13 @@
       </c>
     </row>
     <row r="25" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="15" t="s">
         <v>118</v>
       </c>
@@ -3046,7 +3053,7 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
       <c r="AA25" s="15"/>
-      <c r="AB25" s="42"/>
+      <c r="AB25" s="47"/>
       <c r="AC25" s="22" t="s">
         <v>39</v>
       </c>
@@ -3061,19 +3068,19 @@
       </c>
     </row>
     <row r="26" spans="1:32" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="47">
         <v>3795623</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F26" s="15" t="s">
@@ -3120,7 +3127,7 @@
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
       <c r="AA26" s="15"/>
-      <c r="AB26" s="42" t="s">
+      <c r="AB26" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC26" s="22" t="s">
@@ -3137,13 +3144,13 @@
       </c>
     </row>
     <row r="27" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="15" t="s">
         <v>31</v>
       </c>
@@ -3190,7 +3197,7 @@
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
       <c r="AA27" s="15"/>
-      <c r="AB27" s="42"/>
+      <c r="AB27" s="47"/>
       <c r="AC27" s="22" t="s">
         <v>39</v>
       </c>
@@ -3205,13 +3212,13 @@
       </c>
     </row>
     <row r="28" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="15" t="s">
         <v>118</v>
       </c>
@@ -3260,7 +3267,7 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
       <c r="AA28" s="15"/>
-      <c r="AB28" s="42"/>
+      <c r="AB28" s="47"/>
       <c r="AC28" s="22" t="s">
         <v>39</v>
       </c>
@@ -3275,13 +3282,13 @@
       </c>
     </row>
     <row r="29" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="15" t="s">
         <v>27</v>
       </c>
@@ -3324,7 +3331,7 @@
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
       <c r="AA29" s="15"/>
-      <c r="AB29" s="42"/>
+      <c r="AB29" s="47"/>
       <c r="AC29" s="22" t="s">
         <v>39</v>
       </c>
@@ -3339,13 +3346,13 @@
       </c>
     </row>
     <row r="30" spans="1:32" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="48"/>
       <c r="F30" s="15" t="s">
         <v>118</v>
       </c>
@@ -3394,7 +3401,7 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
       <c r="AA30" s="15"/>
-      <c r="AB30" s="42"/>
+      <c r="AB30" s="47"/>
       <c r="AC30" s="22" t="s">
         <v>39</v>
       </c>
@@ -3809,19 +3816,19 @@
       </c>
     </row>
     <row r="36" spans="1:32" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F36" s="15" t="s">
@@ -3868,7 +3875,7 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
       <c r="AA36" s="15"/>
-      <c r="AB36" s="42" t="s">
+      <c r="AB36" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC36" s="22" t="s">
@@ -3885,13 +3892,13 @@
       </c>
     </row>
     <row r="37" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
       <c r="C37" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
       <c r="F37" s="15" t="s">
         <v>27</v>
       </c>
@@ -3934,7 +3941,7 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
       <c r="AA37" s="15"/>
-      <c r="AB37" s="42"/>
+      <c r="AB37" s="47"/>
       <c r="AC37" s="22" t="s">
         <v>39</v>
       </c>
@@ -4417,19 +4424,19 @@
       </c>
     </row>
     <row r="44" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F44" s="15" t="s">
@@ -4478,7 +4485,7 @@
       <c r="Y44" s="15"/>
       <c r="Z44" s="15"/>
       <c r="AA44" s="15"/>
-      <c r="AB44" s="42" t="s">
+      <c r="AB44" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC44" s="22" t="s">
@@ -4495,13 +4502,13 @@
       </c>
     </row>
     <row r="45" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="50"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
       <c r="F45" s="15" t="s">
         <v>7</v>
       </c>
@@ -4548,7 +4555,7 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
       <c r="AA45" s="15"/>
-      <c r="AB45" s="42"/>
+      <c r="AB45" s="47"/>
       <c r="AC45" s="22" t="s">
         <v>39</v>
       </c>
@@ -4563,13 +4570,13 @@
       </c>
     </row>
     <row r="46" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="43"/>
+      <c r="A46" s="50"/>
+      <c r="B46" s="48"/>
       <c r="C46" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
       <c r="F46" s="15" t="s">
         <v>7</v>
       </c>
@@ -4616,7 +4623,7 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
       <c r="AA46" s="15"/>
-      <c r="AB46" s="42"/>
+      <c r="AB46" s="47"/>
       <c r="AC46" s="22" t="s">
         <v>39</v>
       </c>
@@ -4631,13 +4638,13 @@
       </c>
     </row>
     <row r="47" spans="1:32" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="43"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="48"/>
       <c r="C47" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="15" t="s">
         <v>7</v>
       </c>
@@ -4684,7 +4691,7 @@
       <c r="Y47" s="15"/>
       <c r="Z47" s="15"/>
       <c r="AA47" s="15"/>
-      <c r="AB47" s="42"/>
+      <c r="AB47" s="47"/>
       <c r="AC47" s="22" t="s">
         <v>39</v>
       </c>
@@ -4699,13 +4706,13 @@
       </c>
     </row>
     <row r="48" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="43"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="48"/>
       <c r="C48" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
       <c r="F48" s="15" t="s">
         <v>7</v>
       </c>
@@ -4752,7 +4759,7 @@
       <c r="Y48" s="15"/>
       <c r="Z48" s="15"/>
       <c r="AA48" s="15"/>
-      <c r="AB48" s="42"/>
+      <c r="AB48" s="47"/>
       <c r="AC48" s="22" t="s">
         <v>39</v>
       </c>
@@ -4845,19 +4852,19 @@
       </c>
     </row>
     <row r="50" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="48">
         <v>3795623</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F50" s="15" t="s">
@@ -4908,7 +4915,7 @@
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
       <c r="AA50" s="15"/>
-      <c r="AB50" s="42" t="s">
+      <c r="AB50" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC50" s="22" t="s">
@@ -4925,13 +4932,13 @@
       </c>
     </row>
     <row r="51" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
-      <c r="B51" s="43"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="15" t="s">
         <v>7</v>
       </c>
@@ -4980,7 +4987,7 @@
       <c r="Y51" s="15"/>
       <c r="Z51" s="15"/>
       <c r="AA51" s="15"/>
-      <c r="AB51" s="42"/>
+      <c r="AB51" s="47"/>
       <c r="AC51" s="22" t="s">
         <v>39</v>
       </c>
@@ -4995,13 +5002,13 @@
       </c>
     </row>
     <row r="52" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
-      <c r="B52" s="43"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="48"/>
       <c r="C52" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
       <c r="F52" s="15" t="s">
         <v>7</v>
       </c>
@@ -5050,7 +5057,7 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
       <c r="AA52" s="15"/>
-      <c r="AB52" s="42"/>
+      <c r="AB52" s="47"/>
       <c r="AC52" s="22" t="s">
         <v>39</v>
       </c>
@@ -5065,13 +5072,13 @@
       </c>
     </row>
     <row r="53" spans="1:16364" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
-      <c r="B53" s="43"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="48"/>
       <c r="C53" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
       <c r="F53" s="15" t="s">
         <v>7</v>
       </c>
@@ -5120,7 +5127,7 @@
       <c r="Y53" s="15"/>
       <c r="Z53" s="15"/>
       <c r="AA53" s="15"/>
-      <c r="AB53" s="42"/>
+      <c r="AB53" s="47"/>
       <c r="AC53" s="22" t="s">
         <v>39</v>
       </c>
@@ -5135,19 +5142,19 @@
       </c>
     </row>
     <row r="54" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="43">
+      <c r="D54" s="48">
         <v>3795623</v>
       </c>
-      <c r="E54" s="43" t="s">
+      <c r="E54" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F54" s="15" t="s">
@@ -5198,7 +5205,7 @@
       <c r="Y54" s="15"/>
       <c r="Z54" s="15"/>
       <c r="AA54" s="15"/>
-      <c r="AB54" s="42" t="s">
+      <c r="AB54" s="47" t="s">
         <v>179</v>
       </c>
       <c r="AC54" s="22" t="s">
@@ -5215,13 +5222,13 @@
       </c>
     </row>
     <row r="55" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="48"/>
       <c r="C55" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
       <c r="F55" s="15" t="s">
         <v>7</v>
       </c>
@@ -5270,7 +5277,7 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
       <c r="AA55" s="15"/>
-      <c r="AB55" s="42"/>
+      <c r="AB55" s="47"/>
       <c r="AC55" s="22" t="s">
         <v>39</v>
       </c>
@@ -5285,13 +5292,13 @@
       </c>
     </row>
     <row r="56" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="43"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
       <c r="F56" s="15" t="s">
         <v>7</v>
       </c>
@@ -5340,7 +5347,7 @@
       <c r="Y56" s="15"/>
       <c r="Z56" s="15"/>
       <c r="AA56" s="15"/>
-      <c r="AB56" s="42"/>
+      <c r="AB56" s="47"/>
       <c r="AC56" s="22" t="s">
         <v>39</v>
       </c>
@@ -5355,13 +5362,13 @@
       </c>
     </row>
     <row r="57" spans="1:16364" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
-      <c r="B57" s="43"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="48"/>
       <c r="C57" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
       <c r="F57" s="15" t="s">
         <v>7</v>
       </c>
@@ -5410,7 +5417,7 @@
       <c r="Y57" s="15"/>
       <c r="Z57" s="15"/>
       <c r="AA57" s="15"/>
-      <c r="AB57" s="42"/>
+      <c r="AB57" s="47"/>
       <c r="AC57" s="22" t="s">
         <v>39</v>
       </c>
@@ -5425,13 +5432,13 @@
       </c>
     </row>
     <row r="58" spans="1:16364" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
-      <c r="B58" s="43"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="48"/>
       <c r="C58" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
       <c r="F58" s="15" t="s">
         <v>7</v>
       </c>
@@ -5480,7 +5487,7 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
       <c r="AA58" s="15"/>
-      <c r="AB58" s="42"/>
+      <c r="AB58" s="47"/>
       <c r="AC58" s="22" t="s">
         <v>39</v>
       </c>
@@ -22287,19 +22294,19 @@
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A65" s="42" t="s">
+      <c r="A65" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D65" s="43" t="s">
+      <c r="D65" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E65" s="42" t="s">
+      <c r="E65" s="47" t="s">
         <v>46</v>
       </c>
       <c r="F65" s="15" t="s">
@@ -22363,13 +22370,13 @@
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
-      <c r="B66" s="42"/>
+      <c r="A66" s="47"/>
+      <c r="B66" s="47"/>
       <c r="C66" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D66" s="43"/>
-      <c r="E66" s="42"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="47"/>
       <c r="F66" s="15" t="s">
         <v>7</v>
       </c>
@@ -22431,13 +22438,13 @@
       </c>
     </row>
     <row r="67" spans="1:32" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
-      <c r="B67" s="42"/>
+      <c r="A67" s="47"/>
+      <c r="B67" s="47"/>
       <c r="C67" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D67" s="43"/>
-      <c r="E67" s="42"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="47"/>
       <c r="F67" s="15" t="s">
         <v>31</v>
       </c>
@@ -22501,13 +22508,13 @@
       </c>
     </row>
     <row r="68" spans="1:32" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="42"/>
-      <c r="B68" s="42"/>
+      <c r="A68" s="47"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="43"/>
-      <c r="E68" s="42"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="47"/>
       <c r="F68" s="15" t="s">
         <v>31</v>
       </c>
@@ -22655,19 +22662,19 @@
       </c>
     </row>
     <row r="70" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="43" t="s">
+      <c r="E70" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F70" s="15" t="s">
@@ -22720,7 +22727,7 @@
       <c r="AA70" s="15">
         <v>18</v>
       </c>
-      <c r="AB70" s="42" t="s">
+      <c r="AB70" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC70" s="22" t="s">
@@ -22737,13 +22744,13 @@
       </c>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A71" s="43"/>
-      <c r="B71" s="43"/>
+      <c r="A71" s="48"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
       <c r="F71" s="15" t="s">
         <v>27</v>
       </c>
@@ -22786,7 +22793,7 @@
       <c r="Y71" s="15"/>
       <c r="Z71" s="15"/>
       <c r="AA71" s="15"/>
-      <c r="AB71" s="42"/>
+      <c r="AB71" s="47"/>
       <c r="AC71" s="22" t="s">
         <v>39</v>
       </c>
@@ -22801,19 +22808,19 @@
       </c>
     </row>
     <row r="72" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D72" s="43" t="s">
+      <c r="D72" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="E72" s="43" t="s">
+      <c r="E72" s="48" t="s">
         <v>46</v>
       </c>
       <c r="F72" s="15" t="s">
@@ -22866,7 +22873,7 @@
       <c r="AA72" s="15">
         <v>18</v>
       </c>
-      <c r="AB72" s="42" t="s">
+      <c r="AB72" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AC72" s="22" t="s">
@@ -22883,13 +22890,13 @@
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A73" s="43"/>
-      <c r="B73" s="43"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
       <c r="F73" s="15" t="s">
         <v>27</v>
       </c>
@@ -22932,7 +22939,7 @@
       <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
       <c r="AA73" s="15"/>
-      <c r="AB73" s="42"/>
+      <c r="AB73" s="47"/>
       <c r="AC73" s="22" t="s">
         <v>39</v>
       </c>
@@ -23649,7 +23656,7 @@
         <v>67</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>193</v>
+        <v>42</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>50</v>
@@ -23721,7 +23728,7 @@
         <v>67</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>50</v>
@@ -23839,11 +23846,17 @@
         <v>4534534534</v>
       </c>
       <c r="X85" s="15">
-        <v>130245</v>
-      </c>
-      <c r="Y85" s="15"/>
-      <c r="Z85" s="15"/>
-      <c r="AA85" s="15"/>
+        <v>166152</v>
+      </c>
+      <c r="Y85" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z85" s="15">
+        <v>40</v>
+      </c>
+      <c r="AA85" s="15">
+        <v>40</v>
+      </c>
       <c r="AB85" s="38" t="s">
         <v>44</v>
       </c>
@@ -23862,25 +23875,41 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="AB7:AB10"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="AB3:AB6"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="AB72:AB73"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="AB70:AB71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="AB11:AB14"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AB17:AB20"/>
+    <mergeCell ref="AB21:AB25"/>
+    <mergeCell ref="AB26:AB30"/>
     <mergeCell ref="AB36:AB37"/>
     <mergeCell ref="AB50:AB53"/>
     <mergeCell ref="AB54:AB58"/>
@@ -23897,41 +23926,25 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="AB44:AB48"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="AB11:AB14"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AB17:AB20"/>
-    <mergeCell ref="AB21:AB25"/>
-    <mergeCell ref="AB26:AB30"/>
-    <mergeCell ref="AB72:AB73"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="AB70:AB71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="AB7:AB10"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="AB3:AB6"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AC7" r:id="rId1"/>
@@ -24029,7 +24042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -24042,158 +24055,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
+      <c r="AF1" s="60"/>
     </row>
     <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="50" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>201</v>
-      </c>
-      <c r="I2" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="T2" s="50" t="s">
+      <c r="U2" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="U2" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="V2" s="50" t="s">
+      <c r="V2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="50" t="s">
+      <c r="W2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="50" t="s">
+      <c r="X2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="50" t="s">
+      <c r="Y2" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" s="50" t="s">
+      <c r="Z2" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="50" t="s">
+      <c r="AA2" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="50" t="s">
+      <c r="AB2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="AC2" s="50" t="s">
+      <c r="AC2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="50" t="s">
+      <c r="AD2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="50" t="s">
+      <c r="AE2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="50" t="s">
+      <c r="AF2" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" s="52" t="s">
+      <c r="A3" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54">
+      <c r="C3" s="55"/>
+      <c r="D3" s="58">
         <v>3795623</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="59" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G3" s="57" t="s">
-        <v>203</v>
+        <v>196</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
@@ -24209,42 +24222,42 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="11"/>
-      <c r="V3" s="53">
+      <c r="V3" s="55">
         <v>123566534</v>
       </c>
-      <c r="W3" s="53">
+      <c r="W3" s="55">
         <v>4534534534</v>
       </c>
       <c r="X3" s="11"/>
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="53" t="s">
+      <c r="AB3" s="55" t="s">
         <v>44</v>
       </c>
       <c r="AC3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AD3" s="55" t="s">
+      <c r="AD3" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AE3" s="55" t="s">
+      <c r="AE3" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF3" s="55" t="s">
+      <c r="AF3" s="51" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="52"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59"/>
       <c r="F4" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="58"/>
+        <v>197</v>
+      </c>
+      <c r="G4" s="53"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -24259,37 +24272,37 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="55"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="53"/>
+      <c r="AB4" s="55"/>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="55"/>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="55"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" s="53" t="s">
+      <c r="A5" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54">
+      <c r="C5" s="55"/>
+      <c r="D5" s="58">
         <v>3795623</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="55" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G5" s="57" t="s">
-        <v>203</v>
+        <v>196</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -24305,42 +24318,42 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="53">
+      <c r="V5" s="55">
         <v>123566534</v>
       </c>
-      <c r="W5" s="53">
+      <c r="W5" s="55">
         <v>4534534534</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="53" t="s">
+      <c r="AB5" s="55" t="s">
         <v>179</v>
       </c>
       <c r="AC5" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="AD5" s="55" t="s">
+      <c r="AD5" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AE5" s="55" t="s">
+      <c r="AE5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="55" t="s">
+      <c r="AF5" s="51" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="53"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G6" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="G6" s="54"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -24355,28 +24368,28 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="55"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="53"/>
+      <c r="AB6" s="55"/>
       <c r="AC6" s="56"/>
-      <c r="AD6" s="55"/>
-      <c r="AE6" s="55"/>
-      <c r="AF6" s="55"/>
+      <c r="AD6" s="51"/>
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="51"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="53"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G7" s="58"/>
+        <v>198</v>
+      </c>
+      <c r="G7" s="53"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -24391,37 +24404,37 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="53"/>
+      <c r="AB7" s="55"/>
       <c r="AC7" s="56"/>
-      <c r="AD7" s="55"/>
-      <c r="AE7" s="55"/>
-      <c r="AF7" s="55"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="51"/>
+      <c r="AF7" s="51"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" s="52" t="s">
+      <c r="A8" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="54">
+      <c r="C8" s="55"/>
+      <c r="D8" s="58">
         <v>3795623</v>
       </c>
-      <c r="E8" s="52"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>204</v>
-      </c>
-      <c r="H8" s="57"/>
+        <v>196</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="52"/>
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -24435,43 +24448,43 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="11"/>
-      <c r="V8" s="53">
+      <c r="V8" s="55">
         <v>123566534</v>
       </c>
-      <c r="W8" s="53">
+      <c r="W8" s="55">
         <v>4534534534</v>
       </c>
       <c r="X8" s="11"/>
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="53" t="s">
+      <c r="AB8" s="55" t="s">
         <v>44</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AD8" s="55" t="s">
+      <c r="AD8" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AE8" s="55" t="s">
+      <c r="AE8" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF8" s="55" t="s">
+      <c r="AF8" s="51" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="52"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
+        <v>197</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -24485,38 +24498,38 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="53"/>
-      <c r="W9" s="53"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="53"/>
+      <c r="AB9" s="55"/>
       <c r="AC9" s="1"/>
-      <c r="AD9" s="55"/>
-      <c r="AE9" s="55"/>
-      <c r="AF9" s="55"/>
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" s="53" t="s">
+      <c r="A10" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54">
+      <c r="C10" s="55"/>
+      <c r="D10" s="58">
         <v>3795623</v>
       </c>
-      <c r="E10" s="53"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>204</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>202</v>
+        <v>196</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>201</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -24531,43 +24544,43 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="53">
+      <c r="V10" s="55">
         <v>123566534</v>
       </c>
-      <c r="W10" s="53">
+      <c r="W10" s="55">
         <v>4534534534</v>
       </c>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="53" t="s">
+      <c r="AB10" s="55" t="s">
         <v>179</v>
       </c>
       <c r="AC10" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="AD10" s="55" t="s">
+      <c r="AD10" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AE10" s="55" t="s">
+      <c r="AE10" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF10" s="55" t="s">
+      <c r="AF10" s="51" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="53"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="55"/>
       <c r="F11" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -24581,29 +24594,29 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="53"/>
-      <c r="W11" s="53"/>
+      <c r="V11" s="55"/>
+      <c r="W11" s="55"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="53"/>
+      <c r="AB11" s="55"/>
       <c r="AC11" s="56"/>
-      <c r="AD11" s="55"/>
-      <c r="AE11" s="55"/>
-      <c r="AF11" s="55"/>
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="51"/>
+      <c r="AF11" s="51"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="53"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+        <v>198</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -24617,43 +24630,40 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="53"/>
+      <c r="V12" s="55"/>
+      <c r="W12" s="55"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="53"/>
+      <c r="AB12" s="55"/>
       <c r="AC12" s="56"/>
-      <c r="AD12" s="55"/>
-      <c r="AE12" s="55"/>
-      <c r="AF12" s="55"/>
+      <c r="AD12" s="51"/>
+      <c r="AE12" s="51"/>
+      <c r="AF12" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="AF10:AF12"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="V10:V12"/>
-    <mergeCell ref="W10:W12"/>
-    <mergeCell ref="AB10:AB12"/>
-    <mergeCell ref="AC10:AC12"/>
-    <mergeCell ref="AD10:AD12"/>
-    <mergeCell ref="AE10:AE12"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AE8:AE9"/>
-    <mergeCell ref="AF8:AF9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="AB5:AB7"/>
     <mergeCell ref="AC5:AC7"/>
     <mergeCell ref="AD5:AD7"/>
     <mergeCell ref="AE5:AE7"/>
@@ -24664,26 +24674,29 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="V8:V9"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="W5:W7"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="V10:V12"/>
+    <mergeCell ref="W10:W12"/>
+    <mergeCell ref="AB10:AB12"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AD10:AD12"/>
+    <mergeCell ref="AE10:AE12"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AF8:AF9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AC3" r:id="rId1"/>
@@ -24693,4 +24706,694 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="47">
+        <v>3795623</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="41">
+        <v>123566534</v>
+      </c>
+      <c r="W3" s="15">
+        <v>4534534534</v>
+      </c>
+      <c r="X3" s="15">
+        <v>120696</v>
+      </c>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="41">
+        <v>123566534</v>
+      </c>
+      <c r="W4" s="15">
+        <v>4534534534</v>
+      </c>
+      <c r="X4" s="15">
+        <v>120696</v>
+      </c>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="M5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="41">
+        <v>123566534</v>
+      </c>
+      <c r="W5" s="15">
+        <v>4534534534</v>
+      </c>
+      <c r="X5" s="15">
+        <v>120696</v>
+      </c>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="47"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21"/>
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="21"/>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="21"/>
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" s="15">
+        <v>123456</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="41">
+        <v>123566534</v>
+      </c>
+      <c r="W12" s="15">
+        <v>4534534534</v>
+      </c>
+      <c r="X12" s="15">
+        <v>120696</v>
+      </c>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="47"/>
+      <c r="AC12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD12" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="D3:D12"/>
+    <mergeCell ref="E3:E12"/>
+    <mergeCell ref="AB3:AB12"/>
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AC3" r:id="rId1"/>
+    <hyperlink ref="AC4" r:id="rId2"/>
+    <hyperlink ref="AC5" r:id="rId3"/>
+    <hyperlink ref="AC12" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>